<commit_message>
Put all functions together in a notebook develop for CORE18 paper on HD computing: exploring the storing and retrieval capabilities of binary vectors
</commit_message>
<xml_diff>
--- a/McRaeDataset/FEATS_brm.xlsx
+++ b/McRaeDataset/FEATS_brm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\McRaeDataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA858A90-BED6-40DE-AFB8-4705AFE23720}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E15E148A-0654-4B02-AFB7-2224281DA856}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10211" tabRatio="194" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8663,10 +8663,10 @@
   <dimension ref="A1:J2527"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -81884,7 +81884,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
New small changes to main function, and extended dictionary
</commit_message>
<xml_diff>
--- a/McRaeDataset/FEATS_brm.xlsx
+++ b/McRaeDataset/FEATS_brm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\McRaeDataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E15E148A-0654-4B02-AFB7-2224281DA856}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F28DA3F-DB5F-41AE-8947-09CA8BB4A313}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10211" tabRatio="194" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="features" sheetId="1" r:id="rId1"/>
     <sheet name="variable_explanations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -8663,10 +8663,10 @@
   <dimension ref="A1:J2527"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B329" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomRight" activeCell="A352" activeCellId="1" sqref="A351 A352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>

</xml_diff>